<commit_message>
Changed Attribut to Attribute for consistency
</commit_message>
<xml_diff>
--- a/data/SampleV.01/Elementplan_DE_SampleV.01.xlsx
+++ b/data/SampleV.01/Elementplan_DE_SampleV.01.xlsx
@@ -39,10 +39,10 @@
     <t>Pset</t>
   </si>
   <si>
-    <t>AttributDescriptionDE</t>
-  </si>
-  <si>
-    <t>AttributName</t>
+    <t>AttributeDescriptionDE</t>
+  </si>
+  <si>
+    <t>AttributeName</t>
   </si>
   <si>
     <t>Unit</t>
@@ -120,10 +120,10 @@
     <t>Luftraum</t>
   </si>
   <si>
+    <t>Fenster</t>
+  </si>
+  <si>
     <t>Türen</t>
-  </si>
-  <si>
-    <t>Fenster</t>
   </si>
   <si>
     <t>IfcProject ist der Hauptcontainer für ein digitales Bauprojekt. Es speichert wesentliche Projektinformationen wie:&lt;br&gt;_x005F_x000D_
@@ -175,12 +175,12 @@
     <t>IfcSpace</t>
   </si>
   <si>
+    <t>IfcWindow</t>
+  </si>
+  <si>
     <t>IfcDoor</t>
   </si>
   <si>
-    <t>IfcWindow</t>
-  </si>
-  <si>
     <t>Pset_SpaceCommon</t>
   </si>
   <si>
@@ -196,114 +196,103 @@
     <t>Eindeutige Geschossbezeichnung</t>
   </si>
   <si>
-    <t>Empfehlung:\n_x005F_x000D_
-- Raumkennung: Persistente eindeutige numerische Bezeichnung \n_x005F_x000D_
-- Definition: Ein eindeutiger, dauerhafter numerischer Code, der jedem Raum zur unmissverständlichen Identifizierung innerhalb eines Gebäudes oder Komplexes zugewiesen wird. Z.B. #007 \n_x005F_x000D_
-\n_x005F_x000D_
-Schlüsselprinzipien für effektives Datenmanagement:_x005F_x000D_
-_x005F_x000D_
-1. Beständigkeit: Behalten Sie dieselbe Kennung bei, solange die Kernattribute des Raums unverändert bleiben:_x005F_x000D_
-   - Position (nicht in einen anderen Teil des Gebäudes verlegt)_x005F_x000D_
-   - Allgemeine Größe (geringfügige Anpassungen sind akzeptabel)_x005F_x000D_
-   - Primäre Funktion (z.B. bleibt ein Büro oder Besprechungsraum)_x005F_x000D_
-_x005F_x000D_
-2. Keine Wiederverwendung: Alte Kennungen ausmustern, statt sie neuen Räumen zuzuweisen:_x005F_x000D_
-   - Verhindert Verwirrung bei historischen Datenanalysen_x005F_x000D_
-   - Vermeidet potenzielle Fehler in Facility-Management-Systemen_x005F_x000D_
-_x005F_x000D_
-3. Konsistenz: Kennungen systematisch in allen Gebäudedokumentationen und -systemen anwenden:_x005F_x000D_
-   - Grundrisse_x005F_x000D_
-   - Gebäudeinformationsmodelle (BIM)_x005F_x000D_
-   - Facility-Management-Software_x005F_x000D_
-   - Wartungsaufzeichnungen_x005F_x000D_
-_x005F_x000D_
-4. Formatstandardisierung: Ein einheitliches Format für alle Kennungen verwenden:_x005F_x000D_
-   - Z.B. dreistellige Zahlen mit vorangestelltem # (#001, #002, usw.)_x005F_x000D_
-   - Für größere Komplexe Gebäude- oder Etagenpräfixe in Betracht ziehen (B1-#007, B2-#007)_x005F_x000D_
-_x005F_x000D_
-5. Änderungsmanagement: Einen formalen Prozess für notwendige Kennungsänderungen implementieren:_x005F_x000D_
-   - Gründe für Änderungen dokumentieren_x005F_x000D_
-   - Alle relevanten Systeme und Dokumentationen aktualisieren_x005F_x000D_
-   - Änderungsprotokoll für zukünftige Referenzen führen_x005F_x000D_
-_x005F_x000D_
-6. Kundengetriebenen Änderungen widerstehen: Wenn Kunden während der Projektdurchführung Änderungen der Raumnummerierung wünschen:_x005F_x000D_
-   - Erklären Sie, dass die aktuellen Kennungen technische Raumnummern sind, die für die Datenintegrität entscheidend sind_x005F_x000D_
-   - Bieten Sie an, ein separates, nicht-technisches Raumnummernattribut hinzuzufügen, um ihre Präferenz zu berücksichtigen_x005F_x000D_
-   - Betonen Sie die Wichtigkeit der Beibehaltung der ursprünglichen Kennungen für die Systemkonsistenz und zukünftige Betriebsabläufe_x005F_x000D_
-_x005F_x000D_
+    <t>Empfehlung:\n
+- Raumkennung: Persistente eindeutige numerische Bezeichnung \n
+- Definition: Ein eindeutiger, dauerhafter numerischer Code, der jedem Raum zur unmissverständlichen Identifizierung innerhalb eines Gebäudes oder Komplexes zugewiesen wird. Z.B. #007 \n
+\n
+Schlüsselprinzipien für effektives Datenmanagement:
+1. Beständigkeit: Behalten Sie dieselbe Kennung bei, solange die Kernattribute des Raums unverändert bleiben:
+   - Position (nicht in einen anderen Teil des Gebäudes verlegt)
+   - Allgemeine Größe (geringfügige Anpassungen sind akzeptabel)
+   - Primäre Funktion (z.B. bleibt ein Büro oder Besprechungsraum)
+2. Keine Wiederverwendung: Alte Kennungen ausmustern, statt sie neuen Räumen zuzuweisen:
+   - Verhindert Verwirrung bei historischen Datenanalysen
+   - Vermeidet potenzielle Fehler in Facility-Management-Systemen
+3. Konsistenz: Kennungen systematisch in allen Gebäudedokumentationen und -systemen anwenden:
+   - Grundrisse
+   - Gebäudeinformationsmodelle (BIM)
+   - Facility-Management-Software
+   - Wartungsaufzeichnungen
+4. Formatstandardisierung: Ein einheitliches Format für alle Kennungen verwenden:
+   - Z.B. dreistellige Zahlen mit vorangestelltem # (#001, #002, usw.)
+   - Für größere Komplexe Gebäude- oder Etagenpräfixe in Betracht ziehen (B1-#007, B2-#007)
+5. Änderungsmanagement: Einen formalen Prozess für notwendige Kennungsänderungen implementieren:
+   - Gründe für Änderungen dokumentieren
+   - Alle relevanten Systeme und Dokumentationen aktualisieren
+   - Änderungsprotokoll für zukünftige Referenzen führen
+6. Kundengetriebenen Änderungen widerstehen: Wenn Kunden während der Projektdurchführung Änderungen der Raumnummerierung wünschen:
+   - Erklären Sie, dass die aktuellen Kennungen technische Raumnummern sind, die für die Datenintegrität entscheidend sind
+   - Bieten Sie an, ein separates, nicht-technisches Raumnummernattribut hinzuzufügen, um ihre Präferenz zu berücksichtigen
+   - Betonen Sie die Wichtigkeit der Beibehaltung der ursprünglichen Kennungen für die Systemkonsistenz und zukünftige Betriebsabläufe
 Merke: Auch wenn es verlockend erscheinen mag, Kennungen neu zu organisieren oder wiederzuverwenden, ist die Aufrechterhaltung der Konsistenz über die Zeit entscheidend für ein zuverlässiges langfristiges Datenmanagement und Analysen im Gebäudebetrieb. Technische Raumnummern sollten stabil bleiben, selbst wenn zusätzliche Beschriftungsschemata für den Kundengebrauch eingeführt werden.</t>
   </si>
   <si>
-    <t>Definition: Eine Typbezeichnung für den Raum, z.B. Büro, Besprechungsraum, Labor, Lager._x005F_x000D_
-_x005F_x000D_
-Beste Praktiken:_x005F_x000D_
-1. Verwenden Sie klare, beschreibende Namen (z.B. "Großraumbüro" statt nur "Büro")_x005F_x000D_
-2. Erstellen Sie eine standardisierte Liste von Raumtypen für Ihre Organisation_x005F_x000D_
-3. Vermeiden Sie Abkürzungen oder Codes, die für einige Benutzer unklar sein könnten_x005F_x000D_
-4. Erwägen Sie die Einbeziehung von Untertypen für eine detailliertere Klassifizierung (z.B. "Besprechungsraum - Groß")_x005F_x000D_
-5. Überprüfen und aktualisieren Sie die Benennungskonventionen regelmäßig, um sicherzustellen, dass sie den sich entwickelnden Anforderungen entsprechen_x005F_x000D_
-_x005F_x000D_
+    <t>Definition: Eine Typbezeichnung für den Raum, z.B. Büro, Besprechungsraum, Labor, Lager.
+Beste Praktiken:
+1. Verwenden Sie klare, beschreibende Namen (z.B. "Großraumbüro" statt nur "Büro")
+2. Erstellen Sie eine standardisierte Liste von Raumtypen für Ihre Organisation
+3. Vermeiden Sie Abkürzungen oder Codes, die für einige Benutzer unklar sein könnten
+4. Erwägen Sie die Einbeziehung von Untertypen für eine detailliertere Klassifizierung (z.B. "Besprechungsraum - Groß")
+5. Überprüfen und aktualisieren Sie die Benennungskonventionen regelmäßig, um sicherzustellen, dass sie den sich entwickelnden Anforderungen entsprechen
 Merke: Konsistente und durchdachte Raumtyp-Benennung ist grundlegend für ein effektives Gebäudeinformationsmanagement. Sie unterstützt verbesserte Entscheidungsfindung, Effizienz und langfristige Datennutzbarkeit in verschiedenen Bereichen des Facility Managements, der Energiemodellierung, der Raumnutzung und der Einhaltung von Vorschriften.</t>
   </si>
   <si>
-    <t xml:space="preserve">Empfehlung:_x005F_x000D_
-- Benenne sie einheitlich für einfache Filterung. z.B. Luftraum_x005F_x000D_
+    <t>Im Attribut können Sie festlegen, ob es sich um einen EXTERNEN oder INTERNEN Raum handelt.</t>
+  </si>
+  <si>
+    <t>Das Attribut definiert die Raumlage:
+- True: Außen (z.B. Balkon)
+- False: Innen (z.B. Küche, Parkgarage)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empfehlung:
+- Benenne sie einheitlich für einfache Filterung. z.B. Luftraum
 </t>
   </si>
   <si>
-    <t>Das Attribut definiert die Raumlage:_x005F_x000D_
-- True: Außen (z.B. Balkon)_x005F_x000D_
-- False: Innen (z.B. Küche, Parkgarage)</t>
-  </si>
-  <si>
-    <t>Im Attribut können Sie festlegen, ob es sich um einen EXTERNEN oder INTERNEN Raum handelt.</t>
-  </si>
-  <si>
-    <t>Empfehlung:_x005F_x000D_
-- Fenstertyp über PredefinedType spezifizieren_x005F_x000D_
-_x005F_x000D_
-Übersetzungen:_x005F_x000D_
-- DOOR ... Tür _x005F_x000D_
-- GATE ... Tor _x005F_x000D_
-- TRAPDOOR ... Klappe_x005F_x000D_
-- USERDEFINED ... Benutzerdefiniert_x005F_x000D_
-- NOTDEFINED ... Nicht definiert_x005F_x000D_
-_x005F_x000D_
+    <t xml:space="preserve">Empfehlung:
+- Fenstertyp über PredefinedType spezifizieren
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empfehlung:
+- Türtyp über PredefinedType spezifizieren
+</t>
+  </si>
+  <si>
+    <t>Empfehlung:
+- Fenstertyp über PredefinedType spezifizieren
+Übersetzungen:
+- DOOR ... Tür 
+- GATE ... Tor 
+- TRAPDOOR ... Klappe
+- USERDEFINED ... Benutzerdefiniert
+- NOTDEFINED ... Nicht definiert
 Wenn Userdefined gewählt wurde, sollte im Attribut ObjectType spezifiziert werden.</t>
   </si>
   <si>
-    <t xml:space="preserve">Empfehlung:_x005F_x000D_
-- Fenstertyp über PredefinedType spezifizieren_x005F_x000D_
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empfehlung:_x005F_x000D_
-- Türtyp über PredefinedType spezifizieren_x005F_x000D_
-</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
     <t>LongName</t>
   </si>
   <si>
+    <t>PredefinedType</t>
+  </si>
+  <si>
+    <t>IsInteriorOrExteriorSpace</t>
+  </si>
+  <si>
     <t>IsExternal</t>
   </si>
   <si>
-    <t>PredefinedType</t>
-  </si>
-  <si>
-    <t>IsInteriorOrExteriorSpace</t>
+    <t>EXTERNAL, INTERNAL</t>
+  </si>
+  <si>
+    <t>TRUE, FALSE</t>
   </si>
   <si>
     <t>test</t>
-  </si>
-  <si>
-    <t>TRUE, FALSE</t>
-  </si>
-  <si>
-    <t>EXTERNAL, INTERNAL</t>
   </si>
   <si>
     <t>DOOR, GATE, TRAPDOOR, USERDEFINED, NOTDEFINED</t>
@@ -1190,10 +1179,10 @@
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>44</v>
@@ -1202,7 +1191,7 @@
         <v>54</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>65</v>
@@ -1254,11 +1243,14 @@
       <c r="E9" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="G9" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>66</v>
@@ -1311,13 +1303,13 @@
         <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>30</v>
@@ -1358,25 +1350,22 @@
         <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>30</v>
@@ -1426,10 +1415,7 @@
         <v>57</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>30</v>
@@ -1482,16 +1468,16 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>58</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>30</v>
@@ -1544,16 +1530,19 @@
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>59</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>30</v>
@@ -1612,10 +1601,10 @@
         <v>46</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>30</v>
@@ -2096,7 +2085,7 @@
         <v>74</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>75</v>

</xml_diff>